<commit_message>
added new copper results
</commit_message>
<xml_diff>
--- a/analysis/edcr/out/top_f1/cobalt_shift_new_20_results.xlsx
+++ b/analysis/edcr/out/top_f1/cobalt_shift_new_20_results.xlsx
@@ -833,31 +833,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L6">
-        <v>0.8225806451612904</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="M6">
-        <v>0.6538461538461539</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="N6">
-        <v>0.7285714285714286</v>
+        <v>0.8</v>
       </c>
       <c r="O6">
-        <v>0</v>
+        <v>0.010752688172043</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>0.0714285714285714</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>0.01307189542483659</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>0.1764705882352942</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>0.09803921568627445</v>
       </c>
       <c r="U6" t="s">
         <v>30</v>
@@ -1025,31 +1025,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L9">
-        <v>0.8225806451612904</v>
+        <v>0.8253968253968254</v>
       </c>
       <c r="M9">
-        <v>0.6538461538461539</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="N9">
-        <v>0.7285714285714286</v>
+        <v>0.7375886524822695</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>0.002816180235534982</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>0.01282051282051277</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>0.00901722391084081</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>0.003423591658885664</v>
       </c>
       <c r="S9">
-        <v>0</v>
+        <v>0.01960784313725483</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>0.01237658183840895</v>
       </c>
       <c r="U9" t="s">
         <v>30</v>
@@ -1155,31 +1155,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L11">
-        <v>0.8225806451612904</v>
+        <v>0.8048780487804879</v>
       </c>
       <c r="M11">
-        <v>0.6538461538461539</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="N11">
-        <v>0.7285714285714286</v>
+        <v>0.8250000000000001</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>-0.01770259638080252</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="Q11">
-        <v>0</v>
+        <v>0.09642857142857142</v>
       </c>
       <c r="R11">
-        <v>0</v>
+        <v>-0.02152080344332855</v>
       </c>
       <c r="S11">
-        <v>0</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="T11">
-        <v>0</v>
+        <v>0.1323529411764706</v>
       </c>
       <c r="U11" t="s">
         <v>30</v>
@@ -1477,31 +1477,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L16">
-        <v>0.8225806451612904</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="M16">
-        <v>0.6538461538461539</v>
+        <v>0.7692307692307693</v>
       </c>
       <c r="N16">
-        <v>0.7285714285714286</v>
+        <v>0.8</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>0.010752688172043</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>0.1153846153846154</v>
       </c>
       <c r="Q16">
-        <v>0</v>
+        <v>0.0714285714285714</v>
       </c>
       <c r="R16">
-        <v>0</v>
+        <v>0.01307189542483659</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>0.1764705882352942</v>
       </c>
       <c r="T16">
-        <v>0</v>
+        <v>0.09803921568627445</v>
       </c>
       <c r="U16" t="s">
         <v>30</v>
@@ -1669,31 +1669,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L19">
-        <v>0.8225806451612904</v>
+        <v>0.8253968253968254</v>
       </c>
       <c r="M19">
-        <v>0.6538461538461539</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="N19">
-        <v>0.7285714285714286</v>
+        <v>0.7375886524822695</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>0.002816180235534982</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>0.01282051282051277</v>
       </c>
       <c r="Q19">
-        <v>0</v>
+        <v>0.00901722391084081</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>0.003423591658885664</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>0.01960784313725483</v>
       </c>
       <c r="T19">
-        <v>0</v>
+        <v>0.01237658183840895</v>
       </c>
       <c r="U19" t="s">
         <v>30</v>
@@ -1799,31 +1799,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L21">
-        <v>0.8225806451612904</v>
+        <v>0.8048780487804879</v>
       </c>
       <c r="M21">
-        <v>0.6538461538461539</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="N21">
-        <v>0.7285714285714286</v>
+        <v>0.8250000000000001</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>-0.01770259638080252</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="Q21">
-        <v>0</v>
+        <v>0.09642857142857142</v>
       </c>
       <c r="R21">
-        <v>0</v>
+        <v>-0.02152080344332855</v>
       </c>
       <c r="S21">
-        <v>0</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>0.1323529411764706</v>
       </c>
       <c r="U21" t="s">
         <v>30</v>
@@ -2056,31 +2056,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L25">
-        <v>0.9473684210526315</v>
+        <v>0.9375</v>
       </c>
       <c r="M25">
-        <v>0.2307692307692308</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="N25">
-        <v>0.3711340206185568</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="O25">
-        <v>0.009868421052631526</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <v>0.03846153846153849</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q25">
-        <v>0.05198508444834399</v>
+        <v>0</v>
       </c>
       <c r="R25">
-        <v>0.01052631578947363</v>
+        <v>0</v>
       </c>
       <c r="S25">
-        <v>0.2000000000000002</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T25">
-        <v>0.1628865979381445</v>
+        <v>0</v>
       </c>
       <c r="U25" t="s">
         <v>31</v>
@@ -2121,31 +2121,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L26">
-        <v>0.9473684210526315</v>
+        <v>0.9375</v>
       </c>
       <c r="M26">
-        <v>0.2307692307692308</v>
+        <v>0.1923076923076923</v>
       </c>
       <c r="N26">
-        <v>0.3711340206185568</v>
+        <v>0.3191489361702128</v>
       </c>
       <c r="O26">
-        <v>0.009868421052631526</v>
+        <v>0</v>
       </c>
       <c r="P26">
-        <v>0.03846153846153849</v>
+        <v>2.775557561562891E-17</v>
       </c>
       <c r="Q26">
-        <v>0.05198508444834399</v>
+        <v>0</v>
       </c>
       <c r="R26">
-        <v>0.01052631578947363</v>
+        <v>0</v>
       </c>
       <c r="S26">
-        <v>0.2000000000000002</v>
+        <v>1.443289932012704E-16</v>
       </c>
       <c r="T26">
-        <v>0.1628865979381445</v>
+        <v>0</v>
       </c>
       <c r="U26" t="s">
         <v>31</v>
@@ -2313,31 +2313,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L29">
-        <v>0.9375</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="M29">
-        <v>0.1923076923076923</v>
+        <v>0.2051282051282051</v>
       </c>
       <c r="N29">
-        <v>0.3191489361702128</v>
+        <v>0.3368421052631579</v>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>0.003676470588235281</v>
       </c>
       <c r="P29">
-        <v>2.775557561562891E-17</v>
+        <v>0.01282051282051283</v>
       </c>
       <c r="Q29">
-        <v>0</v>
+        <v>0.0176931690929451</v>
       </c>
       <c r="R29">
-        <v>0</v>
+        <v>0.003921568627450966</v>
       </c>
       <c r="S29">
-        <v>1.443289932012704E-16</v>
+        <v>0.06666666666666672</v>
       </c>
       <c r="T29">
-        <v>0</v>
+        <v>0.05543859649122799</v>
       </c>
       <c r="U29" t="s">
         <v>31</v>
@@ -2765,31 +2765,31 @@
         <v>0.1547619047619048</v>
       </c>
       <c r="L36">
-        <v>0.765625</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="M36">
-        <v>0.6282051282051282</v>
+        <v>0.8205128205128205</v>
       </c>
       <c r="N36">
-        <v>0.6901408450704225</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="O36">
-        <v>0.515625</v>
+        <v>0.4030612244897959</v>
       </c>
       <c r="P36">
-        <v>0.6153846153846154</v>
+        <v>0.8076923076923077</v>
       </c>
       <c r="Q36">
-        <v>0.6657506011679835</v>
+        <v>0.7028824833702881</v>
       </c>
       <c r="R36">
-        <v>2.0625</v>
+        <v>1.612244897959183</v>
       </c>
       <c r="S36">
-        <v>48.00000000000009</v>
+        <v>63.00000000000011</v>
       </c>
       <c r="T36">
-        <v>27.29577464788735</v>
+        <v>28.81818181818184</v>
       </c>
       <c r="U36" t="s">
         <v>32</v>

</xml_diff>